<commit_message>
3 stage pipeline un-tested
</commit_message>
<xml_diff>
--- a/AnalysisOPCodes.xlsx
+++ b/AnalysisOPCodes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdorosh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icrossle\Desktop\pipelineProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="58">
   <si>
     <t>cycles</t>
   </si>
@@ -104,15 +104,6 @@
     <t>Mov4</t>
   </si>
   <si>
-    <t>Fetch</t>
-  </si>
-  <si>
-    <t>Decode</t>
-  </si>
-  <si>
-    <t>Excute</t>
-  </si>
-  <si>
     <t>S3a</t>
   </si>
   <si>
@@ -192,6 +183,21 @@
   </si>
   <si>
     <t>RF2</t>
+  </si>
+  <si>
+    <t>Fetch(stage1)</t>
+  </si>
+  <si>
+    <t>Decode(stage2)</t>
+  </si>
+  <si>
+    <t>Excute(stage3)</t>
+  </si>
+  <si>
+    <t>Stage1</t>
+  </si>
+  <si>
+    <t>Stage1a</t>
   </si>
 </sst>
 </file>
@@ -207,7 +213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,6 +238,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -678,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -686,22 +698,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -722,15 +719,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -779,9 +767,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -792,15 +777,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -818,6 +794,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1098,15 +1113,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:AH17"/>
+  <dimension ref="C2:AH27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" customWidth="1"/>
@@ -1167,835 +1184,986 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
       <c r="AE3" s="3"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="46"/>
-      <c r="AH3" s="47"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="34"/>
+      <c r="AH3" s="35"/>
     </row>
     <row r="4" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="7"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="8" t="s">
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="8" t="s">
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="8" t="s">
+      <c r="L4" s="49"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="9"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="8" t="s">
+      <c r="O4" s="49"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="9"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="8" t="s">
+      <c r="R4" s="49"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="9"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="8" t="s">
+      <c r="U4" s="49"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="8" t="s">
+      <c r="X4" s="49"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="9" t="s">
+      <c r="AA4" s="49"/>
+      <c r="AB4" s="50"/>
+      <c r="AC4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG4" s="44"/>
-      <c r="AH4" s="45"/>
+      <c r="AD4" s="49"/>
+      <c r="AE4" s="49"/>
+      <c r="AF4" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG4" s="46"/>
+      <c r="AH4" s="47"/>
     </row>
     <row r="5" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="14" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="14" t="s">
+      <c r="K5" s="8"/>
+      <c r="L5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="14" t="s">
+      <c r="N5" s="8"/>
+      <c r="O5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="P5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="14" t="s">
+      <c r="Q5" s="8"/>
+      <c r="R5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="15" t="s">
+      <c r="S5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="T5" s="13"/>
-      <c r="U5" s="14" t="s">
+      <c r="T5" s="8"/>
+      <c r="U5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="V5" s="15" t="s">
+      <c r="V5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="W5" s="13"/>
-      <c r="X5" s="14" t="s">
+      <c r="W5" s="8"/>
+      <c r="X5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="15" t="s">
+      <c r="Y5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="14" t="s">
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AB5" s="15" t="s">
+      <c r="AB5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14" t="s">
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AE5" s="14" t="s">
+      <c r="AE5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AF5" s="54"/>
-      <c r="AG5" s="55" t="s">
+      <c r="AF5" s="42"/>
+      <c r="AG5" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="AH5" s="56" t="s">
+      <c r="AH5" s="44" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C6" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="27">
+      <c r="C6" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="19">
         <v>1</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="I6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="J6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="K6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="L6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="M6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="N6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="O6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="P6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="Q6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="R6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="23" t="s">
+      <c r="S6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="Q6" s="23" t="s">
+      <c r="T6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="23" t="s">
+      <c r="U6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="S6" s="23" t="s">
+      <c r="V6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="23" t="s">
+      <c r="W6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="U6" s="23" t="s">
+      <c r="X6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="V6" s="23" t="s">
+      <c r="Y6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="23" t="s">
+      <c r="Z6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="X6" s="23" t="s">
+      <c r="AA6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="Y6" s="23" t="s">
+      <c r="AB6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="Z6" s="23" t="s">
+      <c r="AC6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="AA6" s="23" t="s">
+      <c r="AD6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AB6" s="23" t="s">
+      <c r="AE6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AC6" s="23" t="s">
+      <c r="AF6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="AD6" s="23" t="s">
+      <c r="AG6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AE6" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF6" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG6" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="AH6" s="24" t="s">
+      <c r="AH6" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C7" s="20"/>
-      <c r="D7" s="28">
+      <c r="C7" s="52"/>
+      <c r="D7" s="20">
         <v>2</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16" t="s">
+      <c r="I7" s="11"/>
+      <c r="J7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="K7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16" t="s">
+      <c r="L7" s="11"/>
+      <c r="M7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="N7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16" t="s">
+      <c r="O7" s="11"/>
+      <c r="P7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="Q7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16" t="s">
+      <c r="R7" s="11"/>
+      <c r="S7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="T7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16" t="s">
+      <c r="U7" s="11"/>
+      <c r="V7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="T7" s="16" t="s">
+      <c r="W7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16" t="s">
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="W7" s="16" t="s">
+      <c r="Z7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16" t="s">
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Z7" s="16" t="s">
+      <c r="AC7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="AA7" s="16"/>
-      <c r="AB7" s="16" t="s">
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AC7" s="16" t="s">
+      <c r="AF7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF7" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="25" t="s">
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C8" s="20"/>
-      <c r="D8" s="28">
+      <c r="C8" s="52"/>
+      <c r="D8" s="20">
         <v>3</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16" t="s">
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16" t="s">
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16" t="s">
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16" t="s">
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16" t="s">
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16" t="s">
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="16" t="s">
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="AD8" s="16"/>
-      <c r="AE8" s="16"/>
-      <c r="AF8" s="16" t="s">
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="AG8" s="16"/>
-      <c r="AH8" s="25"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="17"/>
     </row>
     <row r="9" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="21"/>
-      <c r="D9" s="34">
+      <c r="C9" s="53"/>
+      <c r="D9" s="26">
         <v>4</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="25"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="11"/>
+      <c r="AH9" s="17"/>
     </row>
     <row r="10" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="35">
+      <c r="C10" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="27">
         <v>1</v>
       </c>
-      <c r="E10" s="48"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
-      <c r="AG10" s="11"/>
-      <c r="AH10" s="49"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="37"/>
     </row>
     <row r="11" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C11" s="20"/>
-      <c r="D11" s="36">
+      <c r="C11" s="52"/>
+      <c r="D11" s="28">
         <v>2</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
-      <c r="AA11" s="17"/>
-      <c r="AB11" s="17"/>
-      <c r="AC11" s="17"/>
-      <c r="AD11" s="17"/>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="49"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="37"/>
     </row>
     <row r="12" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C12" s="20"/>
-      <c r="D12" s="36">
+      <c r="C12" s="52"/>
+      <c r="D12" s="28">
         <v>3</v>
       </c>
-      <c r="E12" s="48"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="11"/>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11"/>
-      <c r="AH12" s="49"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="37"/>
     </row>
     <row r="13" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="21"/>
-      <c r="D13" s="37">
+      <c r="C13" s="53"/>
+      <c r="D13" s="29">
         <v>4</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17" t="s">
+      <c r="I13" s="12"/>
+      <c r="J13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17" t="s">
+      <c r="L13" s="12"/>
+      <c r="M13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="17" t="s">
+      <c r="N13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17" t="s">
+      <c r="O13" s="12"/>
+      <c r="P13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="Q13" s="17" t="s">
+      <c r="Q13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17" t="s">
+      <c r="R13" s="12"/>
+      <c r="S13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="T13" s="17" t="s">
+      <c r="T13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U13" s="17"/>
-      <c r="V13" s="17" t="s">
+      <c r="U13" s="12"/>
+      <c r="V13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="W13" s="17" t="s">
+      <c r="W13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="X13" s="17"/>
-      <c r="Y13" s="17" t="s">
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="Z13" s="17" t="s">
+      <c r="Z13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AA13" s="17"/>
-      <c r="AB13" s="17" t="s">
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AC13" s="17" t="s">
+      <c r="AC13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AD13" s="17"/>
-      <c r="AE13" s="17" t="s">
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AF13" s="17" t="s">
+      <c r="AF13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AG13" s="17"/>
-      <c r="AH13" s="22" t="s">
+      <c r="AG13" s="12"/>
+      <c r="AH13" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="42">
+      <c r="C14" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="33">
         <v>1</v>
       </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="12"/>
-      <c r="AC14" s="12"/>
-      <c r="AD14" s="12"/>
-      <c r="AE14" s="12"/>
-      <c r="AF14" s="12"/>
-      <c r="AG14" s="12"/>
-      <c r="AH14" s="51"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="39"/>
     </row>
     <row r="15" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-      <c r="D15" s="39">
+      <c r="C15" s="55"/>
+      <c r="D15" s="30">
         <v>2</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18" t="s">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" s="18" t="s">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="N15" s="18" t="s">
+      <c r="L15" s="13"/>
+      <c r="M15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q15" s="18" t="s">
+      <c r="O15" s="13"/>
+      <c r="P15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q15" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="T15" s="18" t="s">
+      <c r="R15" s="13"/>
+      <c r="S15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="T15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="W15" s="18" t="s">
+      <c r="U15" s="13"/>
+      <c r="V15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="W15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z15" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA15" s="18"/>
-      <c r="AB15" s="18"/>
-      <c r="AC15" s="18" t="s">
+      <c r="Z15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE15" s="13"/>
+      <c r="AF15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AD15" s="18" t="s">
+      <c r="AG15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AE15" s="18"/>
-      <c r="AF15" s="12" t="s">
+      <c r="AH15" s="39" t="s">
         <v>52</v>
-      </c>
-      <c r="AG15" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AH15" s="51" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-      <c r="D16" s="40">
+      <c r="C16" s="55"/>
+      <c r="D16" s="31">
         <v>3</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18" t="s">
+      <c r="I16" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="J16" s="13"/>
+      <c r="K16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="L16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18" t="s">
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L16" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18" t="s">
+      <c r="R16" s="13"/>
+      <c r="S16" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="T16" s="18" t="s">
+      <c r="T16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="W16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="W16" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
-      <c r="AC16" s="18" t="s">
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+      <c r="AB16" s="13"/>
+      <c r="AC16" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD16" s="13"/>
+      <c r="AE16" s="13"/>
+      <c r="AF16" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AD16" s="18"/>
-      <c r="AE16" s="18"/>
-      <c r="AF16" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG16" s="12"/>
-      <c r="AH16" s="51"/>
+      <c r="AG16" s="7"/>
+      <c r="AH16" s="39"/>
     </row>
     <row r="17" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="38"/>
-      <c r="D17" s="41">
+      <c r="C17" s="56"/>
+      <c r="D17" s="32">
         <v>4</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26" t="s">
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26" t="s">
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="26" t="s">
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26"/>
-      <c r="W17" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="X17" s="26"/>
-      <c r="Y17" s="26"/>
-      <c r="Z17" s="26"/>
-      <c r="AA17" s="26"/>
-      <c r="AB17" s="26"/>
-      <c r="AC17" s="26"/>
-      <c r="AD17" s="26"/>
-      <c r="AE17" s="26"/>
-      <c r="AF17" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG17" s="52"/>
-      <c r="AH17" s="53" t="s">
-        <v>47</v>
-      </c>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="18"/>
+      <c r="Z17" s="18"/>
+      <c r="AA17" s="18"/>
+      <c r="AB17" s="18"/>
+      <c r="AC17" s="18"/>
+      <c r="AD17" s="18"/>
+      <c r="AE17" s="18"/>
+      <c r="AF17" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG17" s="40"/>
+      <c r="AH17" s="41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="57"/>
+      <c r="Q22" s="57"/>
+      <c r="R22" s="57"/>
+      <c r="S22" s="57"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
+      <c r="Y22" s="57"/>
+    </row>
+    <row r="23" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="57"/>
+      <c r="P23" s="57"/>
+      <c r="Q23" s="57"/>
+      <c r="R23" s="57"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
+      <c r="Y23" s="57"/>
+    </row>
+    <row r="24" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="58"/>
+      <c r="S24" s="58"/>
+      <c r="T24" s="58"/>
+      <c r="U24" s="58"/>
+      <c r="V24" s="58"/>
+      <c r="W24" s="58"/>
+      <c r="X24" s="58"/>
+      <c r="Y24" s="58"/>
+    </row>
+    <row r="25" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="58"/>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="58"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="58"/>
+      <c r="U25" s="58"/>
+      <c r="V25" s="58"/>
+      <c r="W25" s="58"/>
+      <c r="X25" s="58"/>
+      <c r="Y25" s="58"/>
+    </row>
+    <row r="26" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="59"/>
+      <c r="V26" s="59"/>
+      <c r="W26" s="59"/>
+      <c r="X26" s="59"/>
+      <c r="Y26" s="59"/>
+    </row>
+    <row r="27" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="59"/>
+      <c r="S27" s="59"/>
+      <c r="T27" s="59"/>
+      <c r="U27" s="59"/>
+      <c r="V27" s="59"/>
+      <c r="W27" s="59"/>
+      <c r="X27" s="59"/>
+      <c r="Y27" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
     <mergeCell ref="AF4:AH4"/>
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="T4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="599" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>